<commit_message>
Merged the two equity vol Excel workbooks.
</commit_message>
<xml_diff>
--- a/tests/equity-atm-volatility-surface.xlsx
+++ b/tests/equity-atm-volatility-surface.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB43D4-3963-46FB-9371-AE57D337E338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2123D7A1-DDE4-43C9-ACC1-18C8DD5C729E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9360" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="2" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
     <sheet name="vol_surface" sheetId="1" r:id="rId2"/>
+    <sheet name="bootstrapped_vol_surface" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -35,23 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Tenors</t>
   </si>
   <si>
     <t>Quotes</t>
   </si>
+  <si>
+    <t>Scaled Vol</t>
+  </si>
+  <si>
+    <t>Time-Independent Variances</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Bootstrapped Time-Dependent Vols</t>
+  </si>
+  <si>
+    <t>Time-Dependent Variances</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +90,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -85,7 +113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -183,11 +211,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -196,6 +250,17 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8786676B-1177-4D06-B883-E288BDA43606}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,4 +836,410 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111C99B5-D9A9-46C7-8E7B-1F73FD69AC9C}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <f>vol_surface!A2</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="16">
+        <f>vol_surface!B2</f>
+        <v>12.775</v>
+      </c>
+      <c r="D2" s="9">
+        <f>B2/100</f>
+        <v>0.12775</v>
+      </c>
+      <c r="E2" s="10">
+        <f>(D2^2)*A2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="12">
+        <f>D2</f>
+        <v>0.12775</v>
+      </c>
+      <c r="H2" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <f>E2-H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <f>vol_surface!A3</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B3" s="17">
+        <f>vol_surface!B3</f>
+        <v>13.574999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D13" si="0">B3/100</f>
+        <v>0.13574999999999998</v>
+      </c>
+      <c r="E3" s="10">
+        <f>(D3^2)*A3</f>
+        <v>1.5356718749999995E-3</v>
+      </c>
+      <c r="G3" s="12">
+        <f>SQRT((D3^2*A3-H2)/(A3-A2))</f>
+        <v>0.13574999999999998</v>
+      </c>
+      <c r="H3" s="11">
+        <f>H2+(G3^2)*(A3-A2)</f>
+        <v>1.5356718749999995E-3</v>
+      </c>
+      <c r="J3" s="11">
+        <f>E3-H3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <f>vol_surface!A4</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B4" s="17">
+        <f>vol_surface!B4</f>
+        <v>14.275</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.14275000000000002</v>
+      </c>
+      <c r="E4" s="10">
+        <f>(D4^2)*A4</f>
+        <v>3.3962604166666672E-3</v>
+      </c>
+      <c r="G4" s="12">
+        <f>SQRT((D4^2*A4-H3)/(A4-A3))</f>
+        <v>0.14942242970852809</v>
+      </c>
+      <c r="H4" s="11">
+        <f>H3+(G4^2)*(A4-A3)</f>
+        <v>3.3962604166666677E-3</v>
+      </c>
+      <c r="J4" s="11">
+        <f>E4-H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <f>vol_surface!A5</f>
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="17">
+        <f>vol_surface!B5</f>
+        <v>14.55</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.14550000000000002</v>
+      </c>
+      <c r="E5" s="10">
+        <f>(D5^2)*A5</f>
+        <v>5.2925625000000013E-3</v>
+      </c>
+      <c r="G5" s="12">
+        <f>SQRT((D5^2*A5-H4)/(A5-A4))</f>
+        <v>0.15084967683094319</v>
+      </c>
+      <c r="H5" s="11">
+        <f>H4+(G5^2)*(A5-A4)</f>
+        <v>5.2925625000000013E-3</v>
+      </c>
+      <c r="J5" s="11">
+        <f>E5-H5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <f>vol_surface!A6</f>
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="17">
+        <f>vol_surface!B6</f>
+        <v>14.9</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <f>(D6^2)*A6</f>
+        <v>1.1100499999999999E-2</v>
+      </c>
+      <c r="G6" s="12">
+        <f>SQRT((D6^2*A6-H5)/(A6-A5))</f>
+        <v>0.1524196509640407</v>
+      </c>
+      <c r="H6" s="11">
+        <f>H5+(G6^2)*(A6-A5)</f>
+        <v>1.1100499999999999E-2</v>
+      </c>
+      <c r="J6" s="11">
+        <f>E6-H6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <f>vol_surface!A7</f>
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="17">
+        <f>vol_surface!B7</f>
+        <v>15.1</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.151</v>
+      </c>
+      <c r="E7" s="10">
+        <f>(D7^2)*A7</f>
+        <v>1.7100749999999998E-2</v>
+      </c>
+      <c r="G7" s="12">
+        <f>SQRT((D7^2*A7-H6)/(A7-A6))</f>
+        <v>0.15492256130079954</v>
+      </c>
+      <c r="H7" s="11">
+        <f>H6+(G7^2)*(A7-A6)</f>
+        <v>1.7100749999999998E-2</v>
+      </c>
+      <c r="J7" s="11">
+        <f>E7-H7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <f>vol_surface!A8</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="17">
+        <f>vol_surface!B8</f>
+        <v>15.4</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.154</v>
+      </c>
+      <c r="E8" s="10">
+        <f>(D8^2)*A8</f>
+        <v>2.3716000000000001E-2</v>
+      </c>
+      <c r="G8" s="12">
+        <f>SQRT((D8^2*A8-H7)/(A8-A7))</f>
+        <v>0.1626683743079767</v>
+      </c>
+      <c r="H8" s="11">
+        <f>H7+(G8^2)*(A8-A7)</f>
+        <v>2.3716000000000001E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" ref="J4:J13" si="1">E8-H8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <f>vol_surface!A9</f>
+        <v>2</v>
+      </c>
+      <c r="B9" s="17">
+        <f>vol_surface!B9</f>
+        <v>15.45</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1545</v>
+      </c>
+      <c r="E9" s="10">
+        <f>(D9^2)*A9</f>
+        <v>4.7740499999999998E-2</v>
+      </c>
+      <c r="G9" s="12">
+        <f>SQRT((D9^2*A9-H8)/(A9-A8))</f>
+        <v>0.15499838708838229</v>
+      </c>
+      <c r="H9" s="11">
+        <f>H8+(G9^2)*(A9-A8)</f>
+        <v>4.7740499999999991E-2</v>
+      </c>
+      <c r="J9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <f>vol_surface!A10</f>
+        <v>3</v>
+      </c>
+      <c r="B10" s="17">
+        <f>vol_surface!B10</f>
+        <v>15.885</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.15884999999999999</v>
+      </c>
+      <c r="E10" s="10">
+        <f>(D10^2)*A10</f>
+        <v>7.5699967499999993E-2</v>
+      </c>
+      <c r="G10" s="12">
+        <f>SQRT((D10^2*A10-H9)/(A10-A9))</f>
+        <v>0.16721084743520678</v>
+      </c>
+      <c r="H10" s="11">
+        <f>H9+(G10^2)*(A10-A9)</f>
+        <v>7.5699967499999993E-2</v>
+      </c>
+      <c r="J10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <f>vol_surface!A11</f>
+        <v>5</v>
+      </c>
+      <c r="B11" s="17">
+        <f>vol_surface!B11</f>
+        <v>15.945</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.15945000000000001</v>
+      </c>
+      <c r="E11" s="10">
+        <f>(D11^2)*A11</f>
+        <v>0.12712151250000001</v>
+      </c>
+      <c r="G11" s="12">
+        <f>SQRT((D11^2*A11-H10)/(A11-A10))</f>
+        <v>0.160345790403116</v>
+      </c>
+      <c r="H11" s="11">
+        <f>H10+(G11^2)*(A11-A10)</f>
+        <v>0.12712151250000001</v>
+      </c>
+      <c r="J11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <f>vol_surface!A12</f>
+        <v>7</v>
+      </c>
+      <c r="B12" s="17">
+        <f>vol_surface!B12</f>
+        <v>15.12</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1512</v>
+      </c>
+      <c r="E12" s="10">
+        <f>(D12^2)*A12</f>
+        <v>0.16003007999999999</v>
+      </c>
+      <c r="G12" s="12">
+        <f>SQRT((D12^2*A12-H11)/(A12-A11))</f>
+        <v>0.12827425209292781</v>
+      </c>
+      <c r="H12" s="11">
+        <f>H11+(G12^2)*(A12-A11)</f>
+        <v>0.16003007999999999</v>
+      </c>
+      <c r="J12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <f>vol_surface!A13</f>
+        <v>10</v>
+      </c>
+      <c r="B13" s="18">
+        <f>vol_surface!B13</f>
+        <v>15</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="E13" s="10">
+        <f>(D13^2)*A13</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="G13" s="12">
+        <f>SQRT((D13^2*A13-H12)/(A13-A12))</f>
+        <v>0.14716195160434642</v>
+      </c>
+      <c r="H13" s="11">
+        <f>H12+(G13^2)*(A13-A12)</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="J13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test to see what bootstrap vols look like for extreme original vols.
</commit_message>
<xml_diff>
--- a/tests/equity-atm-volatility-surface.xlsx
+++ b/tests/equity-atm-volatility-surface.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2123D7A1-DDE4-43C9-ACC1-18C8DD5C729E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A66A2A-7BE7-401D-8CEB-86A4E94DB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="2" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" firstSheet="1" activeTab="2" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
     <sheet name="vol_surface" sheetId="1" r:id="rId2"/>
-    <sheet name="bootstrapped_vol_surface" sheetId="3" r:id="rId3"/>
+    <sheet name="extreme_vols" sheetId="4" r:id="rId3"/>
+    <sheet name="bootstrapped_vol_surface" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Tenors</t>
   </si>
@@ -581,9 +582,9 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -599,7 +600,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
@@ -608,7 +609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <f>2/12</f>
         <v>0.16666666666666666</v>
@@ -617,7 +618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <f>3/12</f>
         <v>0.25</v>
@@ -626,7 +627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <f>6/12</f>
         <v>0.5</v>
@@ -635,7 +636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <f>9/12</f>
         <v>0.75</v>
@@ -644,7 +645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -652,7 +653,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -660,7 +661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -668,7 +669,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -676,7 +677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -684,7 +685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -706,13 +707,13 @@
       <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -728,7 +729,7 @@
         <v>12.775</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
@@ -738,7 +739,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <f>2/12</f>
         <v>0.16666666666666666</v>
@@ -748,7 +749,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <f>3/12</f>
         <v>0.25</v>
@@ -758,7 +759,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <f>6/12</f>
         <v>0.5</v>
@@ -768,7 +769,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <f>9/12</f>
         <v>0.75</v>
@@ -778,7 +779,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -787,7 +788,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -796,7 +797,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -805,7 +806,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -814,7 +815,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -823,7 +824,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -839,23 +840,148 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB749A6-92C7-4ED9-9062-500112FB2D06}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>12.333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B4" s="4">
+        <v>14.154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <f>6/12</f>
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111C99B5-D9A9-46C7-8E7B-1F73FD69AC9C}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -878,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <f>vol_surface!A2</f>
         <v>0</v>
@@ -892,7 +1018,7 @@
         <v>0.12775</v>
       </c>
       <c r="E2" s="10">
-        <f>(D2^2)*A2</f>
+        <f t="shared" ref="E2:E13" si="0">(D2^2)*A2</f>
         <v>0</v>
       </c>
       <c r="G2" s="12">
@@ -904,11 +1030,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="11">
-        <f>E2-H2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J2:J7" si="1">E2-H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <f>vol_surface!A3</f>
         <v>8.3333333333333329E-2</v>
@@ -918,27 +1044,27 @@
         <v>13.574999999999999</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D13" si="0">B3/100</f>
+        <f t="shared" ref="D3:D13" si="2">B3/100</f>
         <v>0.13574999999999998</v>
       </c>
       <c r="E3" s="10">
-        <f>(D3^2)*A3</f>
+        <f t="shared" si="0"/>
         <v>1.5356718749999995E-3</v>
       </c>
       <c r="G3" s="12">
-        <f>SQRT((D3^2*A3-H2)/(A3-A2))</f>
+        <f t="shared" ref="G3:G13" si="3">SQRT((D3^2*A3-H2)/(A3-A2))</f>
         <v>0.13574999999999998</v>
       </c>
       <c r="H3" s="11">
-        <f>H2+(G3^2)*(A3-A2)</f>
+        <f t="shared" ref="H3:H13" si="4">H2+(G3^2)*(A3-A2)</f>
         <v>1.5356718749999995E-3</v>
       </c>
       <c r="J3" s="11">
-        <f>E3-H3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <f>vol_surface!A4</f>
         <v>0.16666666666666666</v>
@@ -948,27 +1074,27 @@
         <v>14.275</v>
       </c>
       <c r="D4" s="9">
+        <f t="shared" si="2"/>
+        <v>0.14275000000000002</v>
+      </c>
+      <c r="E4" s="10">
         <f t="shared" si="0"/>
-        <v>0.14275000000000002</v>
-      </c>
-      <c r="E4" s="10">
-        <f>(D4^2)*A4</f>
         <v>3.3962604166666672E-3</v>
       </c>
       <c r="G4" s="12">
-        <f>SQRT((D4^2*A4-H3)/(A4-A3))</f>
+        <f t="shared" si="3"/>
         <v>0.14942242970852809</v>
       </c>
       <c r="H4" s="11">
-        <f>H3+(G4^2)*(A4-A3)</f>
+        <f t="shared" si="4"/>
         <v>3.3962604166666677E-3</v>
       </c>
       <c r="J4" s="11">
-        <f>E4-H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <f>vol_surface!A5</f>
         <v>0.25</v>
@@ -978,27 +1104,27 @@
         <v>14.55</v>
       </c>
       <c r="D5" s="9">
+        <f t="shared" si="2"/>
+        <v>0.14550000000000002</v>
+      </c>
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
-        <v>0.14550000000000002</v>
-      </c>
-      <c r="E5" s="10">
-        <f>(D5^2)*A5</f>
         <v>5.2925625000000013E-3</v>
       </c>
       <c r="G5" s="12">
-        <f>SQRT((D5^2*A5-H4)/(A5-A4))</f>
+        <f t="shared" si="3"/>
         <v>0.15084967683094319</v>
       </c>
       <c r="H5" s="11">
-        <f>H4+(G5^2)*(A5-A4)</f>
+        <f t="shared" si="4"/>
         <v>5.2925625000000013E-3</v>
       </c>
       <c r="J5" s="11">
-        <f>E5-H5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <f>vol_surface!A6</f>
         <v>0.5</v>
@@ -1008,27 +1134,27 @@
         <v>14.9</v>
       </c>
       <c r="D6" s="9">
+        <f t="shared" si="2"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="E6" s="10">
-        <f>(D6^2)*A6</f>
         <v>1.1100499999999999E-2</v>
       </c>
       <c r="G6" s="12">
-        <f>SQRT((D6^2*A6-H5)/(A6-A5))</f>
+        <f t="shared" si="3"/>
         <v>0.1524196509640407</v>
       </c>
       <c r="H6" s="11">
-        <f>H5+(G6^2)*(A6-A5)</f>
+        <f t="shared" si="4"/>
         <v>1.1100499999999999E-2</v>
       </c>
       <c r="J6" s="11">
-        <f>E6-H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <f>vol_surface!A7</f>
         <v>0.75</v>
@@ -1038,27 +1164,27 @@
         <v>15.1</v>
       </c>
       <c r="D7" s="9">
+        <f t="shared" si="2"/>
+        <v>0.151</v>
+      </c>
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>0.151</v>
-      </c>
-      <c r="E7" s="10">
-        <f>(D7^2)*A7</f>
         <v>1.7100749999999998E-2</v>
       </c>
       <c r="G7" s="12">
-        <f>SQRT((D7^2*A7-H6)/(A7-A6))</f>
+        <f t="shared" si="3"/>
         <v>0.15492256130079954</v>
       </c>
       <c r="H7" s="11">
-        <f>H6+(G7^2)*(A7-A6)</f>
+        <f t="shared" si="4"/>
         <v>1.7100749999999998E-2</v>
       </c>
       <c r="J7" s="11">
-        <f>E7-H7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <f>vol_surface!A8</f>
         <v>1</v>
@@ -1068,27 +1194,27 @@
         <v>15.4</v>
       </c>
       <c r="D8" s="9">
+        <f t="shared" si="2"/>
+        <v>0.154</v>
+      </c>
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>0.154</v>
-      </c>
-      <c r="E8" s="10">
-        <f>(D8^2)*A8</f>
         <v>2.3716000000000001E-2</v>
       </c>
       <c r="G8" s="12">
-        <f>SQRT((D8^2*A8-H7)/(A8-A7))</f>
+        <f t="shared" si="3"/>
         <v>0.1626683743079767</v>
       </c>
       <c r="H8" s="11">
-        <f>H7+(G8^2)*(A8-A7)</f>
+        <f t="shared" si="4"/>
         <v>2.3716000000000001E-2</v>
       </c>
       <c r="J8" s="11">
-        <f t="shared" ref="J4:J13" si="1">E8-H8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J8:J13" si="5">E8-H8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <f>vol_surface!A9</f>
         <v>2</v>
@@ -1098,27 +1224,27 @@
         <v>15.45</v>
       </c>
       <c r="D9" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1545</v>
+      </c>
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>0.1545</v>
-      </c>
-      <c r="E9" s="10">
-        <f>(D9^2)*A9</f>
         <v>4.7740499999999998E-2</v>
       </c>
       <c r="G9" s="12">
-        <f>SQRT((D9^2*A9-H8)/(A9-A8))</f>
+        <f t="shared" si="3"/>
         <v>0.15499838708838229</v>
       </c>
       <c r="H9" s="11">
-        <f>H8+(G9^2)*(A9-A8)</f>
+        <f t="shared" si="4"/>
         <v>4.7740499999999991E-2</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <f>vol_surface!A10</f>
         <v>3</v>
@@ -1128,27 +1254,27 @@
         <v>15.885</v>
       </c>
       <c r="D10" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15884999999999999</v>
+      </c>
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>0.15884999999999999</v>
-      </c>
-      <c r="E10" s="10">
-        <f>(D10^2)*A10</f>
         <v>7.5699967499999993E-2</v>
       </c>
       <c r="G10" s="12">
-        <f>SQRT((D10^2*A10-H9)/(A10-A9))</f>
+        <f t="shared" si="3"/>
         <v>0.16721084743520678</v>
       </c>
       <c r="H10" s="11">
-        <f>H9+(G10^2)*(A10-A9)</f>
+        <f t="shared" si="4"/>
         <v>7.5699967499999993E-2</v>
       </c>
       <c r="J10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f>vol_surface!A11</f>
         <v>5</v>
@@ -1158,27 +1284,27 @@
         <v>15.945</v>
       </c>
       <c r="D11" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15945000000000001</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>0.15945000000000001</v>
-      </c>
-      <c r="E11" s="10">
-        <f>(D11^2)*A11</f>
         <v>0.12712151250000001</v>
       </c>
       <c r="G11" s="12">
-        <f>SQRT((D11^2*A11-H10)/(A11-A10))</f>
+        <f t="shared" si="3"/>
         <v>0.160345790403116</v>
       </c>
       <c r="H11" s="11">
-        <f>H10+(G11^2)*(A11-A10)</f>
+        <f t="shared" si="4"/>
         <v>0.12712151250000001</v>
       </c>
       <c r="J11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f>vol_surface!A12</f>
         <v>7</v>
@@ -1188,27 +1314,27 @@
         <v>15.12</v>
       </c>
       <c r="D12" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1512</v>
+      </c>
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>0.1512</v>
-      </c>
-      <c r="E12" s="10">
-        <f>(D12^2)*A12</f>
         <v>0.16003007999999999</v>
       </c>
       <c r="G12" s="12">
-        <f>SQRT((D12^2*A12-H11)/(A12-A11))</f>
+        <f t="shared" si="3"/>
         <v>0.12827425209292781</v>
       </c>
       <c r="H12" s="11">
-        <f>H11+(G12^2)*(A12-A11)</f>
+        <f t="shared" si="4"/>
         <v>0.16003007999999999</v>
       </c>
       <c r="J12" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <f>vol_surface!A13</f>
         <v>10</v>
@@ -1218,23 +1344,23 @@
         <v>15</v>
       </c>
       <c r="D13" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="E13" s="10">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="E13" s="10">
-        <f>(D13^2)*A13</f>
         <v>0.22499999999999998</v>
       </c>
       <c r="G13" s="12">
-        <f>SQRT((D13^2*A13-H12)/(A13-A12))</f>
+        <f t="shared" si="3"/>
         <v>0.14716195160434642</v>
       </c>
       <c r="H13" s="11">
-        <f>H12+(G13^2)*(A13-A12)</f>
+        <f t="shared" si="4"/>
         <v>0.22499999999999998</v>
       </c>
       <c r="J13" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added functionality to annotate plot with calling test's name and file name.
</commit_message>
<xml_diff>
--- a/tests/equity-atm-volatility-surface.xlsx
+++ b/tests/equity-atm-volatility-surface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A50DD6-7AF7-4273-8E0A-5AAB568F68A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9989C135-5954-4FE4-ADC3-F1B3A9248570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44760" yWindow="6765" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Tenors</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Interpolated Vol</t>
+  </si>
+  <si>
+    <t>Vols</t>
+  </si>
+  <si>
+    <t>Data for Step-Wise plotting of Bootstrapped Vols</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -254,19 +260,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -291,8 +284,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,189 +326,8 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Bootstrapped Vols</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>bootstrapped_vol_surface!$G$16:$G$38</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2333333333333328E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.3333333333333329E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.16566666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.249</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.499</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.749</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.9990000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.9990000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.9989999999999997</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6.9989999999999997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.9990000000000006</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>bootstrapped_vol_surface!$H$16:$H$38</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00000</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>0.12775</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12775</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13574999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13574999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.14942242970852809</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14942242970852809</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.15084967683094319</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.15084967683094319</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1524196509640407</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1524196509640407</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.15492256130079954</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.15492256130079954</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.1626683743079767</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.1626683743079767</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.15499838708838229</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.15499838708838229</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.16721084743520678</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.16721084743520678</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.160345790403116</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.160345790403116</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.12827425209292781</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.12827425209292781</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.14716195160434642</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8DDC-46EF-9814-019DE9A7A8B8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:v>Original Vols</c:v>
           </c:tx>
@@ -623,6 +437,187 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8DDC-46EF-9814-019DE9A7A8B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Bootstrapped Vols</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>bootstrapped_vol_surface!$G$18:$G$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2333333333333328E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16566666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.749</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.9990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9989999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9989999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.9990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>bootstrapped_vol_surface!$H$18:$H$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.12775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13574999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13574999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14942242970852809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14942242970852809</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15084967683094319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15084967683094319</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1524196509640407</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1524196509640407</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15492256130079954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15492256130079954</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1626683743079767</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1626683743079767</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15499838708838229</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15499838708838229</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16721084743520678</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.16721084743520678</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.160345790403116</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.160345790403116</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.12827425209292781</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12827425209292781</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.14716195160434642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8DDC-46EF-9814-019DE9A7A8B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -659,6 +654,36 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -704,7 +729,7 @@
         <c:axId val="1505305343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.12000000000000001"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -722,7 +747,37 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00000" sourceLinked="1"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -771,6 +826,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1375,16 +1461,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1976,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B879A-C57C-42F3-85D1-F3C6B382A708}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,14 +2117,14 @@
         <v>0.12775</v>
       </c>
       <c r="D2" s="9">
-        <f>C2^2*A2</f>
+        <f t="shared" ref="D2:D13" si="0">C2^2*A2</f>
         <v>0</v>
       </c>
       <c r="F2" s="12">
         <v>0</v>
       </c>
       <c r="G2" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F2,OFFSET($D$2:$D$13,MATCH(F2,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F2,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ref="G2:G23" ca="1" si="1">_xlfn.FORECAST.LINEAR(F2,OFFSET($D$2:$D$13,MATCH(F2,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F2,$A$2:$A$13,1)-1,0, 2, 1))</f>
         <v>1.0842021724855044E-19</v>
       </c>
       <c r="H2" s="12"/>
@@ -2053,11 +2139,11 @@
         <v>13.574999999999999</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C13" si="0">B3/100</f>
+        <f t="shared" ref="C3:C13" si="2">B3/100</f>
         <v>0.13574999999999998</v>
       </c>
       <c r="D3" s="9">
-        <f>C3^2*A3</f>
+        <f t="shared" si="0"/>
         <v>1.5356718749999995E-3</v>
       </c>
       <c r="F3" s="12">
@@ -2065,7 +2151,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G3" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F3,OFFSET($D$2:$D$13,MATCH(F3,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F3,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7.6783593749999975E-4</v>
       </c>
       <c r="H3" s="12">
@@ -2084,22 +2170,22 @@
         <v>14.275</v>
       </c>
       <c r="C4" s="12">
+        <f t="shared" si="2"/>
+        <v>0.14275000000000002</v>
+      </c>
+      <c r="D4" s="9">
         <f t="shared" si="0"/>
-        <v>0.14275000000000002</v>
-      </c>
-      <c r="D4" s="9">
-        <f>C4^2*A4</f>
         <v>3.3962604166666672E-3</v>
       </c>
       <c r="F4" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G4" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F4,OFFSET($D$2:$D$13,MATCH(F4,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F4,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.5356718749999993E-3</v>
       </c>
       <c r="H4" s="12">
-        <f t="shared" ref="H4:H24" ca="1" si="1">SQRT(G4/F4)</f>
+        <f t="shared" ref="H4:H24" ca="1" si="3">SQRT(G4/F4)</f>
         <v>0.13574999999999998</v>
       </c>
       <c r="I4" s="12"/>
@@ -2114,11 +2200,11 @@
         <v>14.55</v>
       </c>
       <c r="C5" s="12">
+        <f t="shared" si="2"/>
+        <v>0.14550000000000002</v>
+      </c>
+      <c r="D5" s="9">
         <f t="shared" si="0"/>
-        <v>0.14550000000000002</v>
-      </c>
-      <c r="D5" s="9">
-        <f>C5^2*A5</f>
         <v>5.2925625000000013E-3</v>
       </c>
       <c r="F5" s="12">
@@ -2126,11 +2212,11 @@
         <v>0.125</v>
       </c>
       <c r="G5" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F5,OFFSET($D$2:$D$13,MATCH(F5,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F5,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.4659661458333332E-3</v>
       </c>
       <c r="H5" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14045543480644196</v>
       </c>
       <c r="I5" s="12"/>
@@ -2145,22 +2231,22 @@
         <v>14.9</v>
       </c>
       <c r="C6" s="12">
+        <f t="shared" si="2"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D6" s="9">
         <f t="shared" si="0"/>
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="D6" s="9">
-        <f>C6^2*A6</f>
         <v>1.1100499999999999E-2</v>
       </c>
       <c r="F6" s="12">
         <v>0.16666666666666666</v>
       </c>
       <c r="G6" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F6,OFFSET($D$2:$D$13,MATCH(F6,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F6,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3.3962604166666672E-3</v>
       </c>
       <c r="H6" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14275000000000002</v>
       </c>
       <c r="I6" s="12"/>
@@ -2175,11 +2261,11 @@
         <v>15.1</v>
       </c>
       <c r="C7" s="12">
+        <f t="shared" si="2"/>
+        <v>0.151</v>
+      </c>
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>0.151</v>
-      </c>
-      <c r="D7" s="9">
-        <f>C7^2*A7</f>
         <v>1.7100749999999998E-2</v>
       </c>
       <c r="F7" s="12">
@@ -2187,11 +2273,11 @@
         <v>0.20833333333333331</v>
       </c>
       <c r="G7" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F7,OFFSET($D$2:$D$13,MATCH(F7,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F7,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>4.3444114583333342E-3</v>
       </c>
       <c r="H7" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14440628448928394</v>
       </c>
       <c r="I7" s="12"/>
@@ -2205,22 +2291,22 @@
         <v>15.4</v>
       </c>
       <c r="C8" s="12">
+        <f t="shared" si="2"/>
+        <v>0.154</v>
+      </c>
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>0.154</v>
-      </c>
-      <c r="D8" s="9">
-        <f>C8^2*A8</f>
         <v>2.3716000000000001E-2</v>
       </c>
       <c r="F8" s="12">
         <v>0.25</v>
       </c>
       <c r="G8" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F8,OFFSET($D$2:$D$13,MATCH(F8,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F8,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>5.2925625000000013E-3</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14550000000000002</v>
       </c>
       <c r="I8" s="12"/>
@@ -2233,11 +2319,11 @@
         <v>15.45</v>
       </c>
       <c r="C9" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1545</v>
+      </c>
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>0.1545</v>
-      </c>
-      <c r="D9" s="9">
-        <f>C9^2*A9</f>
         <v>4.7740499999999998E-2</v>
       </c>
       <c r="F9" s="12">
@@ -2245,11 +2331,11 @@
         <v>0.375</v>
       </c>
       <c r="G9" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F9,OFFSET($D$2:$D$13,MATCH(F9,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F9,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>8.1965312499999998E-3</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14784254011165618</v>
       </c>
       <c r="I9" s="12"/>
@@ -2262,22 +2348,22 @@
         <v>15.885</v>
       </c>
       <c r="C10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.15884999999999999</v>
+      </c>
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
-        <v>0.15884999999999999</v>
-      </c>
-      <c r="D10" s="9">
-        <f>C10^2*A10</f>
         <v>7.5699967499999993E-2</v>
       </c>
       <c r="F10" s="12">
         <v>0.5</v>
       </c>
       <c r="G10" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F10,OFFSET($D$2:$D$13,MATCH(F10,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F10,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.1100499999999999E-2</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.14899999999999999</v>
       </c>
       <c r="I10" s="12"/>
@@ -2290,11 +2376,11 @@
         <v>15.945</v>
       </c>
       <c r="C11" s="12">
+        <f t="shared" si="2"/>
+        <v>0.15945000000000001</v>
+      </c>
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
-        <v>0.15945000000000001</v>
-      </c>
-      <c r="D11" s="9">
-        <f>C11^2*A11</f>
         <v>0.12712151250000001</v>
       </c>
       <c r="F11" s="12">
@@ -2302,11 +2388,11 @@
         <v>0.625</v>
       </c>
       <c r="G11" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F11,OFFSET($D$2:$D$13,MATCH(F11,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F11,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.4100624999999999E-2</v>
       </c>
       <c r="H11" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15020319570501819</v>
       </c>
       <c r="I11" s="12"/>
@@ -2319,22 +2405,22 @@
         <v>15.12</v>
       </c>
       <c r="C12" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1512</v>
+      </c>
+      <c r="D12" s="9">
         <f t="shared" si="0"/>
-        <v>0.1512</v>
-      </c>
-      <c r="D12" s="9">
-        <f>C12^2*A12</f>
         <v>0.16003007999999999</v>
       </c>
       <c r="F12" s="12">
         <v>0.75</v>
       </c>
       <c r="G12" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F12,OFFSET($D$2:$D$13,MATCH(F12,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F12,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1.7100749999999998E-2</v>
       </c>
       <c r="H12" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.151</v>
       </c>
       <c r="I12" s="12"/>
@@ -2347,11 +2433,11 @@
         <v>15</v>
       </c>
       <c r="C13" s="12">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="D13" s="9">
-        <f>C13^2*A13</f>
         <v>0.22499999999999998</v>
       </c>
       <c r="F13" s="12">
@@ -2359,11 +2445,11 @@
         <v>0.875</v>
       </c>
       <c r="G13" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F13,OFFSET($D$2:$D$13,MATCH(F13,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F13,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.0408374999999999E-2</v>
       </c>
       <c r="H13" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15272150190086903</v>
       </c>
       <c r="I13" s="12"/>
@@ -2373,11 +2459,11 @@
         <v>1</v>
       </c>
       <c r="G14" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F14,OFFSET($D$2:$D$13,MATCH(F14,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F14,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2.3716000000000008E-2</v>
       </c>
       <c r="H14" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15400000000000003</v>
       </c>
       <c r="I14" s="12"/>
@@ -2388,11 +2474,11 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F15,OFFSET($D$2:$D$13,MATCH(F15,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F15,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3.5728250000000003E-2</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15433351331882952</v>
       </c>
       <c r="I15" s="12"/>
@@ -2402,11 +2488,11 @@
         <v>2</v>
       </c>
       <c r="G16" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F16,OFFSET($D$2:$D$13,MATCH(F16,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F16,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>4.7740499999999991E-2</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.1545</v>
       </c>
       <c r="I16" s="12"/>
@@ -2417,11 +2503,11 @@
         <v>2.5</v>
       </c>
       <c r="G17" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F17,OFFSET($D$2:$D$13,MATCH(F17,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F17,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>6.1720233749999992E-2</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15712445226634841</v>
       </c>
       <c r="I17" s="12"/>
@@ -2431,11 +2517,11 @@
         <v>3</v>
       </c>
       <c r="G18" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F18,OFFSET($D$2:$D$13,MATCH(F18,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F18,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>7.5699967499999993E-2</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15884999999999999</v>
       </c>
       <c r="I18" s="12"/>
@@ -2446,11 +2532,11 @@
         <v>4</v>
       </c>
       <c r="G19" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F19,OFFSET($D$2:$D$13,MATCH(F19,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F19,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.10141074</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15922526495503156</v>
       </c>
       <c r="I19" s="12"/>
@@ -2460,11 +2546,11 @@
         <v>5</v>
       </c>
       <c r="G20" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F20,OFFSET($D$2:$D$13,MATCH(F20,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F20,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.12712151250000001</v>
       </c>
       <c r="H20" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15945000000000001</v>
       </c>
       <c r="I20" s="12"/>
@@ -2475,11 +2561,11 @@
         <v>6</v>
       </c>
       <c r="G21" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F21,OFFSET($D$2:$D$13,MATCH(F21,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F21,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.14357579625</v>
       </c>
       <c r="H21" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15469098026387965</v>
       </c>
       <c r="I21" s="12"/>
@@ -2489,11 +2575,11 @@
         <v>7</v>
       </c>
       <c r="G22" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F22,OFFSET($D$2:$D$13,MATCH(F22,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F22,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.16003007999999996</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15119999999999997</v>
       </c>
       <c r="I22" s="12"/>
@@ -2504,11 +2590,11 @@
         <v>8.5</v>
       </c>
       <c r="G23" s="12">
-        <f ca="1">_xlfn.FORECAST.LINEAR(F23,OFFSET($D$2:$D$13,MATCH(F23,$A$2:$A$13,1)-1,0, 2, 1),OFFSET($A$2:$A$13,MATCH(F23,$A$2:$A$13,1)-1,0, 2, 1))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0.19251503999999997</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0.15049527645509048</v>
       </c>
       <c r="I23" s="12"/>
@@ -2522,16 +2608,16 @@
         <v>0.22499999999999998</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="I24" s="12"/>
     </row>
     <row r="32" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="K32" s="20"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="20"/>
+      <c r="K33" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2666,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111C99B5-D9A9-46C7-8E7B-1F73FD69AC9C}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="C3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,6 +2829,10 @@
         <f>vol_surface!B3</f>
         <v>13.574999999999999</v>
       </c>
+      <c r="C3">
+        <f>A3*360</f>
+        <v>30</v>
+      </c>
       <c r="D3" s="9">
         <f t="shared" ref="D3:D13" si="2">B3/100</f>
         <v>0.13574999999999998</v>
@@ -2773,6 +2863,10 @@
         <f>vol_surface!B4</f>
         <v>14.275</v>
       </c>
+      <c r="C4">
+        <f>A4*360</f>
+        <v>60</v>
+      </c>
       <c r="D4" s="9">
         <f t="shared" si="2"/>
         <v>0.14275000000000002</v>
@@ -2803,6 +2897,10 @@
         <f>vol_surface!B5</f>
         <v>14.55</v>
       </c>
+      <c r="C5">
+        <f>A5*360</f>
+        <v>90</v>
+      </c>
       <c r="D5" s="9">
         <f t="shared" si="2"/>
         <v>0.14550000000000002</v>
@@ -2833,6 +2931,10 @@
         <f>vol_surface!B6</f>
         <v>14.9</v>
       </c>
+      <c r="C6">
+        <f>A6*360</f>
+        <v>180</v>
+      </c>
       <c r="D6" s="9">
         <f t="shared" si="2"/>
         <v>0.14899999999999999</v>
@@ -3064,210 +3166,222 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="15">
+      <c r="G16" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H17" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
         <v>0.12775</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="19">
-        <f>G18-0.001</f>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="12">
+        <f>G20-0.001</f>
         <v>8.2333333333333328E-2</v>
-      </c>
-      <c r="H17" s="12">
-        <f>H16</f>
-        <v>0.12775</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G18" s="6">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H18" s="12">
-        <v>0.13574999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G19" s="19">
-        <f>G20-0.001</f>
-        <v>0.16566666666666666</v>
       </c>
       <c r="H19" s="12">
         <f>H18</f>
+        <v>0.12775</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="12">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H20" s="12">
         <v>0.13574999999999998</v>
       </c>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G20" s="6">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0.14942242970852809</v>
-      </c>
-    </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G21" s="19">
+      <c r="G21" s="12">
         <f>G22-0.001</f>
-        <v>0.249</v>
+        <v>0.16566666666666666</v>
       </c>
       <c r="H21" s="12">
         <f>H20</f>
+        <v>0.13574999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="12">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H22" s="12">
         <v>0.14942242970852809</v>
       </c>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0.15084967683094319</v>
-      </c>
-    </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="19">
+      <c r="G23" s="12">
         <f>G24-0.001</f>
-        <v>0.499</v>
+        <v>0.249</v>
       </c>
       <c r="H23" s="12">
         <f>H22</f>
+        <v>0.14942242970852809</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="H24" s="12">
         <v>0.15084967683094319</v>
       </c>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0.1524196509640407</v>
-      </c>
-    </row>
     <row r="25" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G25" s="19">
+      <c r="G25" s="12">
         <f>G26-0.001</f>
-        <v>0.749</v>
+        <v>0.499</v>
       </c>
       <c r="H25" s="12">
         <f>H24</f>
+        <v>0.15084967683094319</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="12">
         <v>0.1524196509640407</v>
       </c>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="H26" s="12">
-        <v>0.15492256130079954</v>
-      </c>
-    </row>
     <row r="27" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="19">
+      <c r="G27" s="12">
         <f>G28-0.001</f>
-        <v>0.999</v>
+        <v>0.749</v>
       </c>
       <c r="H27" s="12">
         <f>H26</f>
+        <v>0.1524196509640407</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="H28" s="12">
         <v>0.15492256130079954</v>
       </c>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="6">
-        <v>1</v>
-      </c>
-      <c r="H28" s="12">
-        <v>0.1626683743079767</v>
-      </c>
-    </row>
     <row r="29" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="19">
+      <c r="G29" s="12">
         <f>G30-0.001</f>
-        <v>1.9990000000000001</v>
+        <v>0.999</v>
       </c>
       <c r="H29" s="12">
         <f>H28</f>
+        <v>0.15492256130079954</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12">
         <v>0.1626683743079767</v>
       </c>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G30" s="6">
-        <v>2</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0.15499838708838229</v>
-      </c>
-    </row>
     <row r="31" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G31" s="19">
+      <c r="G31" s="12">
         <f>G32-0.001</f>
-        <v>2.9990000000000001</v>
+        <v>1.9990000000000001</v>
       </c>
       <c r="H31" s="12">
         <f>H30</f>
+        <v>0.1626683743079767</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="12">
+        <v>2</v>
+      </c>
+      <c r="H32" s="12">
         <v>0.15499838708838229</v>
       </c>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G32" s="6">
-        <v>3</v>
-      </c>
-      <c r="H32" s="12">
-        <v>0.16721084743520678</v>
-      </c>
-    </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" s="19">
+      <c r="G33" s="12">
         <f>G34-0.001</f>
-        <v>4.9989999999999997</v>
+        <v>2.9990000000000001</v>
       </c>
       <c r="H33" s="12">
         <f>H32</f>
+        <v>0.15499838708838229</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="12">
+        <v>3</v>
+      </c>
+      <c r="H34" s="12">
         <v>0.16721084743520678</v>
       </c>
     </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" s="6">
-        <v>5</v>
-      </c>
-      <c r="H34" s="12">
-        <v>0.160345790403116</v>
-      </c>
-    </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G35" s="19">
+      <c r="G35" s="12">
         <f>G36-0.001</f>
-        <v>6.9989999999999997</v>
+        <v>4.9989999999999997</v>
       </c>
       <c r="H35" s="12">
         <f>H34</f>
+        <v>0.16721084743520678</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="12">
+        <v>5</v>
+      </c>
+      <c r="H36" s="12">
         <v>0.160345790403116</v>
       </c>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="6">
-        <v>7</v>
-      </c>
-      <c r="H36" s="12">
-        <v>0.12827425209292781</v>
-      </c>
-    </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="19">
+      <c r="G37" s="12">
         <f>G38-0.001</f>
-        <v>9.9990000000000006</v>
+        <v>6.9989999999999997</v>
       </c>
       <c r="H37" s="12">
         <f>H36</f>
+        <v>0.160345790403116</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="12">
+        <v>7</v>
+      </c>
+      <c r="H38" s="12">
         <v>0.12827425209292781</v>
       </c>
     </row>
-    <row r="38" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="7">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G39" s="12">
+        <f>G40-0.001</f>
+        <v>9.9990000000000006</v>
+      </c>
+      <c r="H39" s="12">
+        <f>H38</f>
+        <v>0.12827425209292781</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G40" s="12">
         <v>10</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H40" s="12">
         <v>0.14716195160434642</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the vol time to maturity for extreme volatilities to 1 in step sizes of 0.1
</commit_message>
<xml_diff>
--- a/tests/equity-atm-volatility-surface.xlsx
+++ b/tests/equity-atm-volatility-surface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3CE9E9-0D75-47B5-AADC-0BDBB4A7DB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B31507-467D-4663-8C17-AF28D431B63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
@@ -2658,7 +2658,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2673,15 +2673,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="B3" s="4">
         <v>22</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>2</v>
+        <v>0.3</v>
       </c>
       <c r="B4" s="4">
         <v>29</v>
@@ -2697,15 +2697,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="B5" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="4">
         <v>42</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="B7" s="4">
         <v>50</v>
@@ -2721,23 +2721,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <v>6</v>
+        <v>0.7</v>
       </c>
       <c r="B8" s="4">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>7</v>
+      <c r="A9" s="21">
+        <v>0.8</v>
       </c>
       <c r="B9" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="21">
-        <v>8</v>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7">
+        <v>0.9</v>
       </c>
       <c r="B10" s="22">
         <v>77</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" s="5">
         <v>95</v>

</xml_diff>

<commit_message>
Added test_simulate_time_dependent_gbm_with_periodic_vols and test_simulate_time_dependent_gbm_with_annual_vols Plots.
</commit_message>
<xml_diff>
--- a/tests/equity-atm-volatility-surface.xlsx
+++ b/tests/equity-atm-volatility-surface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B31507-467D-4663-8C17-AF28D431B63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5169D3-62AC-4737-9B21-0A3070EBE11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="linear_variance_interpolation" sheetId="5" r:id="rId3"/>
     <sheet name="extreme_vols" sheetId="4" r:id="rId4"/>
     <sheet name="bootstrapped_vol_surface" sheetId="3" r:id="rId5"/>
+    <sheet name="annual_vols" sheetId="6" r:id="rId6"/>
+    <sheet name="stepwise_vols" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Tenors</t>
   </si>
@@ -2657,8 +2659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB749A6-92C7-4ED9-9062-500112FB2D06}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3397,4 +3399,210 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D439AE-F2EE-47F9-9F95-C0D2F698AB6A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF5E9B7-513C-4EBC-A494-C0F7368C5D98}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>